<commit_message>
Atualizada ATA e grafico do Project Charter
</commit_message>
<xml_diff>
--- a/Banco de Dados de PADS/TRE_Dados_MapaRaciocinio.xlsx
+++ b/Banco de Dados de PADS/TRE_Dados_MapaRaciocinio.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Atas das Reuniões" sheetId="5" r:id="rId3"/>
     <sheet name="PROCESSO PADRÃO" sheetId="4" r:id="rId4"/>
     <sheet name="Controle do Projeto" sheetId="6" r:id="rId5"/>
-    <sheet name="ÁREAS PADRÃO" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -69,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="199">
   <si>
     <t>Categoria</t>
   </si>
@@ -642,9 +641,6 @@
   </si>
   <si>
     <t>Secretaria de Gestão de Serviços</t>
-  </si>
-  <si>
-    <t>Coordenadoria de InfraEstrutura Predial</t>
   </si>
   <si>
     <t>Coordenadoria de Segurança , Transporte e Apoio Administrativo</t>
@@ -704,6 +700,25 @@
   </si>
   <si>
     <t>Média de Coordenadoria de Segurança e Transportes e Apoio Administrativo</t>
+  </si>
+  <si>
+    <t>Ivis , Ruhan , Andre , Silmara, Iva , Helcio, Joao Paulo(Flavio), Helcio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentado modelo A0;
+Apresentada a fase do Measure e suas ferramentas;
+Solicitado o volume da PADS para Ivanilda para criar comparitivo de custos atuais e futuros(Tempo e Dinheiro);
+Sugerida a possibilidade de levantamento de tempo gasto por servidor por PAD com base nos 37 pads coletados;
+</t>
+  </si>
+  <si>
+    <t>*Alterar imagens do Step 4 para ver as novas medias;
+*Alterar legendas  da planilha de custos para contemplar PADS;
+*Ajustar casas decimais dos graficos do Project Charter;
+*Verificar se e possivel obter o numero de servidores da CIP , ASSISEG para retirar o custo medio por servidor baseado na hora de cada tramite;</t>
+  </si>
+  <si>
+    <t>Ruhan, Ivis e Andre</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1635,6 +1650,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1660,27 +1684,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1702,8 +1726,8 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1738,7 +1762,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1780,7 +1803,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1991,11 +2013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1310694288"/>
-        <c:axId val="1310701360"/>
+        <c:axId val="384306744"/>
+        <c:axId val="384305568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1310694288"/>
+        <c:axId val="384306744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,7 +2037,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1310701360"/>
+        <c:crossAx val="384305568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2023,7 +2045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1310701360"/>
+        <c:axId val="384305568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1310694288"/>
+        <c:crossAx val="384306744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2246,11 +2268,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="1310694832"/>
-        <c:axId val="1310695376"/>
+        <c:axId val="384304392"/>
+        <c:axId val="384304000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1310694832"/>
+        <c:axId val="384304392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,7 +2282,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1310695376"/>
+        <c:crossAx val="384304000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2268,7 +2290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1310695376"/>
+        <c:axId val="384304000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2279,7 +2301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1310694832"/>
+        <c:crossAx val="384304392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2509,11 +2531,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="1133839856"/>
-        <c:axId val="1133840400"/>
+        <c:axId val="384303216"/>
+        <c:axId val="384302824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1133839856"/>
+        <c:axId val="384303216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2545,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1133840400"/>
+        <c:crossAx val="384302824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2531,7 +2553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1133840400"/>
+        <c:axId val="384302824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2542,7 +2564,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1133839856"/>
+        <c:crossAx val="384303216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3021,16 +3043,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>38102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:rowOff>97972</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3041,8 +3063,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7372351" y="962027"/>
-          <a:ext cx="1181100" cy="47624"/>
+          <a:off x="7375071" y="941616"/>
+          <a:ext cx="1224643" cy="59870"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3178,6 +3200,92 @@
         </a:prstGeom>
         <a:solidFill>
           <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0C0C0" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="22"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>8856</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>117021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>566058</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>162740</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7383927" y="1020535"/>
+          <a:ext cx="1776402" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>389856</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>89807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65315</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>135526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8984127" y="1183821"/>
+          <a:ext cx="285059" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="12"/>
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
@@ -3507,12 +3615,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
       <c r="E1" s="95" t="s">
         <v>9</v>
       </c>
@@ -3521,7 +3629,7 @@
       </c>
       <c r="G1" s="97">
         <f ca="1">TODAY()</f>
-        <v>42850</v>
+        <v>42852</v>
       </c>
       <c r="H1" s="98" t="s">
         <v>11</v>
@@ -3568,7 +3676,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="107" t="s">
         <v>111</v>
@@ -3607,7 +3715,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" s="107" t="s">
         <v>127</v>
@@ -3637,7 +3745,7 @@
         <v>129</v>
       </c>
       <c r="B6" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>127</v>
@@ -3667,7 +3775,7 @@
         <v>131</v>
       </c>
       <c r="B7" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="107" t="s">
         <v>127</v>
@@ -3697,7 +3805,7 @@
         <v>132</v>
       </c>
       <c r="B8" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="107" t="s">
         <v>127</v>
@@ -3727,7 +3835,7 @@
         <v>133</v>
       </c>
       <c r="B9" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="107" t="s">
         <v>127</v>
@@ -3755,7 +3863,7 @@
         <v>134</v>
       </c>
       <c r="B10" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="107" t="s">
         <v>127</v>
@@ -3782,7 +3890,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="107" t="s">
         <v>111</v>
@@ -3809,7 +3917,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" s="107" t="s">
         <v>111</v>
@@ -3835,12 +3943,12 @@
       <c r="A13" s="116"/>
       <c r="B13" s="107"/>
       <c r="C13" s="117"/>
-      <c r="D13" s="134" t="s">
-        <v>195</v>
-      </c>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
+      <c r="D13" s="137" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="137"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="138"/>
       <c r="H13" s="108">
         <f>AVERAGE(H4:H12)</f>
         <v>169.66666666666666</v>
@@ -4029,7 +4137,7 @@
       <c r="F20" s="126">
         <v>42135</v>
       </c>
-      <c r="G20" s="153">
+      <c r="G20" s="134">
         <v>42171</v>
       </c>
       <c r="H20" s="108">
@@ -4389,15 +4497,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="136" t="s">
         <v>181</v>
       </c>
-      <c r="B34" s="134"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="135"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="137"/>
+      <c r="F34" s="137"/>
+      <c r="G34" s="138"/>
       <c r="H34" s="108">
         <f>AVERAGE(H14:H33)</f>
         <v>173.05</v>
@@ -4622,7 +4730,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'ÁREAS PADRÃO'!$A$1:$A$3</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B4:B33</xm:sqref>
         </x14:dataValidation>
@@ -4637,7 +4745,7 @@
   <dimension ref="A2:J148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4704,7 +4812,7 @@
         <v>184</v>
       </c>
       <c r="E5" s="1">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4742,104 +4850,104 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="136" t="s">
+      <c r="C17" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="138"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="141"/>
+      <c r="G19" s="141"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="141"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="141"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="141"/>
+      <c r="G22" s="141"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="138"/>
+      <c r="C23" s="141"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="141"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
+      <c r="E24" s="141"/>
+      <c r="F24" s="141"/>
+      <c r="G24" s="141"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="141"/>
+      <c r="F25" s="141"/>
+      <c r="G25" s="141"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
+      <c r="G26" s="141"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="141"/>
+      <c r="G27" s="141"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="138"/>
-      <c r="D28" s="138"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="141"/>
+      <c r="G29" s="141"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="141"/>
+      <c r="F30" s="141"/>
+      <c r="G30" s="141"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="80" t="s">
@@ -5491,7 +5599,8 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5541,7 +5650,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="45" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="139">
+      <c r="A2" s="143">
         <v>1</v>
       </c>
       <c r="B2" s="142" t="s">
@@ -5571,7 +5680,7 @@
       <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="140"/>
+      <c r="A3" s="144"/>
       <c r="B3" s="142"/>
       <c r="C3" s="142"/>
       <c r="D3" s="142"/>
@@ -5603,7 +5712,7 @@
       <c r="D4" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="139">
+      <c r="E4" s="143">
         <v>2</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -5621,11 +5730,11 @@
       <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="140"/>
+      <c r="A5" s="143"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="144"/>
       <c r="F5" s="37" t="s">
         <v>54</v>
       </c>
@@ -5644,16 +5753,16 @@
       <c r="A6" s="142">
         <v>3</v>
       </c>
-      <c r="B6" s="143">
+      <c r="B6" s="146">
         <v>42683</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="139" t="s">
+      <c r="D6" s="143" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="139">
+      <c r="E6" s="143">
         <v>2</v>
       </c>
       <c r="F6" s="31" t="s">
@@ -5672,10 +5781,10 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="142"/>
-      <c r="B7" s="140"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
       <c r="F7" s="55" t="s">
         <v>67</v>
       </c>
@@ -5692,10 +5801,10 @@
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="142"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="140"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="144"/>
       <c r="F8" s="53" t="s">
         <v>69</v>
       </c>
@@ -5712,10 +5821,10 @@
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="142"/>
-      <c r="B9" s="140"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
       <c r="F9" s="53" t="s">
         <v>73</v>
       </c>
@@ -5732,10 +5841,10 @@
     </row>
     <row r="10" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="142"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="147"/>
       <c r="F10" s="31" t="s">
         <v>70</v>
       </c>
@@ -5803,11 +5912,11 @@
       <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="139"/>
-      <c r="B13" s="139"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="139"/>
+      <c r="A13" s="143"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="143"/>
+      <c r="E13" s="143"/>
       <c r="F13" s="70" t="s">
         <v>72</v>
       </c>
@@ -5823,17 +5932,17 @@
       <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="139">
+      <c r="A14" s="143">
         <v>5</v>
       </c>
-      <c r="B14" s="143">
+      <c r="B14" s="146">
         <v>42705</v>
       </c>
-      <c r="C14" s="139"/>
-      <c r="D14" s="139" t="s">
+      <c r="C14" s="143"/>
+      <c r="D14" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="139">
+      <c r="E14" s="143">
         <v>2</v>
       </c>
       <c r="F14" s="71" t="s">
@@ -5851,11 +5960,11 @@
       <c r="J14" s="67"/>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
-      <c r="B15" s="144"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="140"/>
-      <c r="E15" s="140"/>
+      <c r="A15" s="144"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
       <c r="F15" s="71" t="s">
         <v>120</v>
       </c>
@@ -5871,11 +5980,11 @@
       <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
-      <c r="B16" s="144"/>
-      <c r="C16" s="140"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="140"/>
+      <c r="A16" s="144"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="144"/>
       <c r="F16" s="71" t="s">
         <v>122</v>
       </c>
@@ -5891,13 +6000,13 @@
       <c r="J16" s="67"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="140"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="140"/>
+      <c r="A17" s="144"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="144"/>
       <c r="D17" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="140"/>
+      <c r="E17" s="144"/>
       <c r="F17" s="71" t="s">
         <v>123</v>
       </c>
@@ -5913,13 +6022,13 @@
       <c r="J17" s="67"/>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="144"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="139" t="s">
+      <c r="A18" s="144"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="143" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="140"/>
+      <c r="E18" s="144"/>
       <c r="F18" s="71" t="s">
         <v>125</v>
       </c>
@@ -5935,11 +6044,11 @@
       <c r="J18" s="67"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="140"/>
-      <c r="B19" s="144"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
+      <c r="A19" s="144"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="144"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="142">
@@ -6011,7 +6120,7 @@
         <v>180</v>
       </c>
       <c r="G23" s="127" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H23" s="127"/>
       <c r="I23" s="130" t="s">
@@ -6027,30 +6136,57 @@
         <v>42809</v>
       </c>
       <c r="C24" s="127" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="127">
         <v>2</v>
       </c>
       <c r="F24" s="129" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24" s="127" t="s">
         <v>190</v>
       </c>
-      <c r="G24" s="127" t="s">
+      <c r="H24" s="127" t="s">
         <v>191</v>
-      </c>
-      <c r="H24" s="127" t="s">
-        <v>192</v>
       </c>
       <c r="I24" s="58" t="s">
         <v>57</v>
       </c>
       <c r="J24" s="127"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="125"/>
+    <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A25" s="132">
+        <v>8</v>
+      </c>
+      <c r="B25" s="133">
+        <v>42852</v>
+      </c>
+      <c r="C25" s="132" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="132" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="132">
+        <v>2</v>
+      </c>
+      <c r="F25" s="156" t="s">
+        <v>197</v>
+      </c>
+      <c r="G25" s="132" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" s="133">
+        <v>42863</v>
+      </c>
+      <c r="I25" s="130" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="132"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F26" s="125"/>
@@ -6063,6 +6199,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="E20:E23"/>
@@ -6079,21 +6230,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6104,7 +6240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -6271,8 +6407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6281,20 +6417,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="150" t="s">
+      <c r="C1" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151" t="s">
+      <c r="D1" s="154"/>
+      <c r="E1" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="152"/>
+      <c r="F1" s="155"/>
       <c r="G1" s="15" t="s">
         <v>35</v>
       </c>
@@ -6314,8 +6450,8 @@
       <c r="U1" s="16"/>
     </row>
     <row r="2" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
-      <c r="B2" s="149"/>
+      <c r="A2" s="150"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="17" t="s">
         <v>36</v>
       </c>
@@ -6451,10 +6587,18 @@
       <c r="B5" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
+      <c r="C5" s="28">
+        <v>42794</v>
+      </c>
+      <c r="D5" s="29">
+        <v>42825</v>
+      </c>
+      <c r="E5" s="29">
+        <v>42737</v>
+      </c>
+      <c r="F5" s="30">
+        <v>42851</v>
+      </c>
       <c r="G5" s="26"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
@@ -6478,9 +6622,15 @@
       <c r="B6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="28">
+        <v>42857</v>
+      </c>
+      <c r="D6" s="29">
+        <v>42886</v>
+      </c>
+      <c r="E6" s="29">
+        <v>42852</v>
+      </c>
       <c r="F6" s="30"/>
       <c r="G6" s="26"/>
       <c r="H6" s="31"/>
@@ -6506,7 +6656,9 @@
         <v>42</v>
       </c>
       <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
+      <c r="D7" s="29">
+        <v>43008</v>
+      </c>
       <c r="E7" s="29"/>
       <c r="F7" s="30"/>
       <c r="G7" s="26"/>
@@ -6533,7 +6685,9 @@
         <v>43</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
+      <c r="D8" s="29">
+        <v>43069</v>
+      </c>
       <c r="E8" s="29"/>
       <c r="F8" s="30"/>
       <c r="G8" s="26"/>
@@ -6560,7 +6714,9 @@
         <v>44</v>
       </c>
       <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
+      <c r="D9" s="29">
+        <v>42794</v>
+      </c>
       <c r="E9" s="29"/>
       <c r="F9" s="30"/>
       <c r="G9" s="26"/>
@@ -6772,37 +6928,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="65.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>